<commit_message>
Most up to date version
</commit_message>
<xml_diff>
--- a/VB_Species_Lookup.xlsx
+++ b/VB_Species_Lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelrund/Dropbox/_NDpostdoc/DataInjestion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A529D713-447B-C541-A7A1-DFE76E717297}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E0576F-743B-A144-9D6E-AB3746D66F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="speciesKeySheet" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3373" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3430" uniqueCount="1112">
   <si>
     <t>Aedes</t>
   </si>
@@ -3306,13 +3307,82 @@
   </si>
   <si>
     <t>Psorophora varipes</t>
+  </si>
+  <si>
+    <t>Anopheles arabiensis</t>
+  </si>
+  <si>
+    <t>VBsp:0002224</t>
+  </si>
+  <si>
+    <t>An. arabiensis</t>
+  </si>
+  <si>
+    <t>VBsp:0003235</t>
+  </si>
+  <si>
+    <t>An arabiensis</t>
+  </si>
+  <si>
+    <t>An. coluzzii</t>
+  </si>
+  <si>
+    <t>An coluzzii</t>
+  </si>
+  <si>
+    <t>Anoopheles coluzzii</t>
+  </si>
+  <si>
+    <t>VBsp:0003829</t>
+  </si>
+  <si>
+    <t>Anopheles gambiae sensu stricto</t>
+  </si>
+  <si>
+    <t>Anopheles gambiae ss</t>
+  </si>
+  <si>
+    <t>An. gambiae ss</t>
+  </si>
+  <si>
+    <t>An gambiae ss</t>
+  </si>
+  <si>
+    <t>VBsp:0003830</t>
+  </si>
+  <si>
+    <t>Anopheles melas</t>
+  </si>
+  <si>
+    <t>VBsp:0003532</t>
+  </si>
+  <si>
+    <t>An melas</t>
+  </si>
+  <si>
+    <t>An. melas</t>
+  </si>
+  <si>
+    <t>Anopheles coluzzii</t>
+  </si>
+  <si>
+    <t>Anopheles stephensi</t>
+  </si>
+  <si>
+    <t>VBsp:0003601</t>
+  </si>
+  <si>
+    <t>An. pharoensis</t>
+  </si>
+  <si>
+    <t>An. stephensi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3365,6 +3435,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FFD1D2D3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3389,10 +3479,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3403,11 +3494,224 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="49">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3967,8 +4271,8 @@
   <dimension ref="A1:G767"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A671" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G690" sqref="G690"/>
+      <pane ySplit="1" topLeftCell="A680" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H688" sqref="H688"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18782,175 +19086,289 @@
       </c>
       <c r="G685" s="2"/>
     </row>
-    <row r="686" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="686" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A686" s="2"/>
       <c r="B686" s="2"/>
-      <c r="C686" s="2"/>
-      <c r="D686" s="2"/>
+      <c r="C686" s="10" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D686" s="11" t="s">
+        <v>1090</v>
+      </c>
       <c r="E686" s="2"/>
-      <c r="F686" s="2"/>
+      <c r="F686" s="10" t="s">
+        <v>1091</v>
+      </c>
       <c r="G686" s="2"/>
     </row>
-    <row r="687" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="687" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A687" s="2"/>
       <c r="B687" s="2"/>
-      <c r="C687" s="2"/>
-      <c r="D687" s="2"/>
+      <c r="C687" s="10" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D687" s="11" t="s">
+        <v>1090</v>
+      </c>
       <c r="E687" s="2"/>
-      <c r="F687" s="2"/>
+      <c r="F687" s="10" t="s">
+        <v>1089</v>
+      </c>
       <c r="G687" s="2"/>
     </row>
-    <row r="688" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="688" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A688" s="2"/>
       <c r="B688" s="2"/>
-      <c r="C688" s="2"/>
-      <c r="D688" s="2"/>
+      <c r="C688" s="10" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D688" s="11" t="s">
+        <v>1090</v>
+      </c>
       <c r="E688" s="2"/>
-      <c r="F688" s="2"/>
+      <c r="F688" s="10" t="s">
+        <v>1093</v>
+      </c>
       <c r="G688" s="2"/>
     </row>
-    <row r="689" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="689" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A689" s="2"/>
       <c r="B689" s="2"/>
-      <c r="C689" s="2"/>
-      <c r="D689" s="2"/>
+      <c r="C689" s="2" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D689" s="11" t="s">
+        <v>1092</v>
+      </c>
       <c r="E689" s="2"/>
-      <c r="F689" s="2"/>
+      <c r="F689" s="2" t="s">
+        <v>1094</v>
+      </c>
       <c r="G689" s="2"/>
     </row>
-    <row r="690" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="690" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A690" s="2"/>
       <c r="B690" s="2"/>
-      <c r="C690" s="2"/>
-      <c r="D690" s="2"/>
+      <c r="C690" s="2" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D690" s="11" t="s">
+        <v>1092</v>
+      </c>
       <c r="E690" s="2"/>
-      <c r="F690" s="2"/>
+      <c r="F690" s="2" t="s">
+        <v>1095</v>
+      </c>
       <c r="G690" s="2"/>
     </row>
-    <row r="691" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="691" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A691" s="2"/>
       <c r="B691" s="2"/>
-      <c r="C691" s="2"/>
-      <c r="D691" s="2"/>
+      <c r="C691" s="2" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D691" s="11" t="s">
+        <v>1092</v>
+      </c>
       <c r="E691" s="2"/>
-      <c r="F691" s="2"/>
+      <c r="F691" s="2" t="s">
+        <v>1096</v>
+      </c>
       <c r="G691" s="2"/>
     </row>
-    <row r="692" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="692" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A692" s="2"/>
       <c r="B692" s="2"/>
-      <c r="C692" s="2"/>
-      <c r="D692" s="2"/>
+      <c r="C692" s="11" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D692" s="11" t="s">
+        <v>1097</v>
+      </c>
       <c r="E692" s="2"/>
-      <c r="F692" s="2"/>
+      <c r="F692" s="11" t="s">
+        <v>1098</v>
+      </c>
       <c r="G692" s="2"/>
     </row>
-    <row r="693" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="693" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A693" s="2"/>
       <c r="B693" s="2"/>
-      <c r="C693" s="2"/>
-      <c r="D693" s="2"/>
+      <c r="C693" s="11" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D693" s="11" t="s">
+        <v>1097</v>
+      </c>
       <c r="E693" s="2"/>
-      <c r="F693" s="2"/>
+      <c r="F693" s="11" t="s">
+        <v>1099</v>
+      </c>
       <c r="G693" s="2"/>
     </row>
-    <row r="694" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="694" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A694" s="2"/>
       <c r="B694" s="2"/>
-      <c r="C694" s="2"/>
-      <c r="D694" s="2"/>
+      <c r="C694" s="11" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D694" s="11" t="s">
+        <v>1097</v>
+      </c>
       <c r="E694" s="2"/>
-      <c r="F694" s="2"/>
+      <c r="F694" s="11" t="s">
+        <v>1100</v>
+      </c>
       <c r="G694" s="2"/>
     </row>
-    <row r="695" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="695" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A695" s="2"/>
       <c r="B695" s="2"/>
-      <c r="C695" s="2"/>
-      <c r="D695" s="2"/>
+      <c r="C695" s="11" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D695" s="11" t="s">
+        <v>1102</v>
+      </c>
       <c r="E695" s="2"/>
-      <c r="F695" s="2"/>
+      <c r="F695" s="11" t="s">
+        <v>1101</v>
+      </c>
       <c r="G695" s="2"/>
     </row>
-    <row r="696" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="696" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A696" s="2"/>
       <c r="B696" s="2"/>
-      <c r="C696" s="2"/>
-      <c r="D696" s="2"/>
+      <c r="C696" s="2" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D696" s="11" t="s">
+        <v>1104</v>
+      </c>
       <c r="E696" s="2"/>
-      <c r="F696" s="2"/>
+      <c r="F696" s="2" t="s">
+        <v>1103</v>
+      </c>
       <c r="G696" s="2"/>
     </row>
-    <row r="697" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="697" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A697" s="2"/>
       <c r="B697" s="2"/>
-      <c r="C697" s="2"/>
-      <c r="D697" s="2"/>
+      <c r="C697" s="2" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D697" s="11" t="s">
+        <v>1104</v>
+      </c>
       <c r="E697" s="2"/>
-      <c r="F697" s="2"/>
+      <c r="F697" s="2" t="s">
+        <v>1105</v>
+      </c>
       <c r="G697" s="2"/>
     </row>
-    <row r="698" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="698" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A698" s="2"/>
       <c r="B698" s="2"/>
-      <c r="C698" s="2"/>
-      <c r="D698" s="2"/>
+      <c r="C698" s="2" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D698" s="11" t="s">
+        <v>1104</v>
+      </c>
       <c r="E698" s="2"/>
-      <c r="F698" s="2"/>
+      <c r="F698" s="2" t="s">
+        <v>1106</v>
+      </c>
       <c r="G698" s="2"/>
     </row>
     <row r="699" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A699" s="2"/>
       <c r="B699" s="2"/>
-      <c r="C699" s="2"/>
-      <c r="D699" s="2"/>
+      <c r="C699" s="2" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D699" s="2" t="s">
+        <v>1090</v>
+      </c>
       <c r="E699" s="2"/>
-      <c r="F699" s="2"/>
+      <c r="F699" s="2" t="s">
+        <v>1089</v>
+      </c>
       <c r="G699" s="2"/>
     </row>
     <row r="700" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A700" s="2"/>
       <c r="B700" s="2"/>
-      <c r="C700" s="2"/>
-      <c r="D700" s="2"/>
+      <c r="C700" s="2" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D700" s="2" t="s">
+        <v>1065</v>
+      </c>
       <c r="E700" s="2"/>
-      <c r="F700" s="2"/>
+      <c r="F700" s="2" t="s">
+        <v>1066</v>
+      </c>
       <c r="G700" s="2"/>
     </row>
     <row r="701" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A701" s="2"/>
       <c r="B701" s="2"/>
-      <c r="C701" s="2"/>
-      <c r="D701" s="2"/>
+      <c r="C701" s="2" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D701" s="2" t="s">
+        <v>1109</v>
+      </c>
       <c r="E701" s="2"/>
-      <c r="F701" s="2"/>
+      <c r="F701" s="2" t="s">
+        <v>1108</v>
+      </c>
       <c r="G701" s="2"/>
     </row>
     <row r="702" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A702" s="2"/>
       <c r="B702" s="2"/>
-      <c r="C702" s="2"/>
-      <c r="D702" s="2"/>
+      <c r="C702" s="2" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D702" s="2" t="s">
+        <v>1090</v>
+      </c>
       <c r="E702" s="2"/>
-      <c r="F702" s="2"/>
+      <c r="F702" s="2" t="s">
+        <v>1091</v>
+      </c>
       <c r="G702" s="2"/>
     </row>
     <row r="703" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A703" s="2"/>
       <c r="B703" s="2"/>
-      <c r="C703" s="2"/>
-      <c r="D703" s="2"/>
+      <c r="C703" s="2" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D703" s="2" t="s">
+        <v>1065</v>
+      </c>
       <c r="E703" s="2"/>
-      <c r="F703" s="2"/>
+      <c r="F703" s="2" t="s">
+        <v>1110</v>
+      </c>
       <c r="G703" s="2"/>
     </row>
     <row r="704" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A704" s="2"/>
       <c r="B704" s="2"/>
-      <c r="C704" s="2"/>
-      <c r="D704" s="2"/>
+      <c r="C704" s="2" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D704" s="2" t="s">
+        <v>1109</v>
+      </c>
       <c r="E704" s="2"/>
-      <c r="F704" s="2"/>
+      <c r="F704" s="2" t="s">
+        <v>1111</v>
+      </c>
       <c r="G704" s="2"/>
     </row>
     <row r="705" spans="1:7" x14ac:dyDescent="0.2">
@@ -19521,90 +19939,162 @@
       <c r="G767" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1048476:F1048576 F529 F430:F502 F351:F428 F190:F203 F675 F1 F7:F154 F180:F188 F157:F176 F178 F205:F349 F504:F520 F686:F1048472">
-    <cfRule type="duplicateValues" dxfId="27" priority="51"/>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <conditionalFormatting sqref="F1048476:F1048576 F529 F430:F502 F351:F428 F190:F203 F675 F1 F7:F154 F180:F188 F157:F176 F178 F205:F349 F504:F520 F689:F691 F705:F1048472">
+    <cfRule type="duplicateValues" dxfId="48" priority="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F429">
-    <cfRule type="duplicateValues" dxfId="26" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F350">
-    <cfRule type="duplicateValues" dxfId="25" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F189">
-    <cfRule type="duplicateValues" dxfId="24" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="69"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F675 F1 F7:F154 F180:F203 F157:F176 F178 F205:F502 F686:F1048576 F504:F671">
-    <cfRule type="duplicateValues" dxfId="23" priority="45"/>
+  <conditionalFormatting sqref="F675 F1 F7:F154 F180:F203 F157:F176 F178 F205:F502 F504:F671 F689:F691 F705:F1048576">
+    <cfRule type="duplicateValues" dxfId="44" priority="66"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F675 F1 F7:F154 F180:F203 F157:F176 F178 F205:F502 F686:F1048576 F504:F672">
-    <cfRule type="duplicateValues" dxfId="22" priority="44"/>
+  <conditionalFormatting sqref="F675 F1 F7:F154 F180:F203 F157:F176 F178 F205:F502 F504:F672 F689:F691 F705:F1048576">
+    <cfRule type="duplicateValues" dxfId="43" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C672">
-    <cfRule type="duplicateValues" dxfId="21" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="64"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F675 F180:F203 F1 F7:F154 F157:F176 F178 F205:F502 F686:F1048576 F504:F673">
-    <cfRule type="duplicateValues" dxfId="20" priority="42"/>
+  <conditionalFormatting sqref="F675 F180:F203 F1 F7:F154 F157:F176 F178 F205:F502 F504:F673 F689:F691 F705:F1048576">
+    <cfRule type="duplicateValues" dxfId="41" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C673">
-    <cfRule type="duplicateValues" dxfId="19" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="62"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F675 F180:F203 F6:F154 F1:F3 F157:F176 F178 F205:F502 F686:F1048576 F504:F673">
-    <cfRule type="duplicateValues" dxfId="18" priority="28"/>
+  <conditionalFormatting sqref="F675 F180:F203 F6:F154 F1:F3 F157:F176 F178 F205:F502 F504:F673 F689:F691 F705:F1048576">
+    <cfRule type="duplicateValues" dxfId="39" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F179">
-    <cfRule type="duplicateValues" dxfId="17" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F179">
-    <cfRule type="duplicateValues" dxfId="16" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F179">
-    <cfRule type="duplicateValues" dxfId="15" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F179">
-    <cfRule type="duplicateValues" dxfId="14" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F179">
-    <cfRule type="duplicateValues" dxfId="13" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C491">
-    <cfRule type="duplicateValues" dxfId="12" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C491">
-    <cfRule type="duplicateValues" dxfId="11" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C491">
-    <cfRule type="duplicateValues" dxfId="10" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C491">
-    <cfRule type="duplicateValues" dxfId="9" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C491">
-    <cfRule type="duplicateValues" dxfId="8" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F503">
-    <cfRule type="duplicateValues" dxfId="7" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F503">
-    <cfRule type="duplicateValues" dxfId="6" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F503">
-    <cfRule type="duplicateValues" dxfId="5" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F503">
-    <cfRule type="duplicateValues" dxfId="4" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F503">
-    <cfRule type="duplicateValues" dxfId="3" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="29"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F680 F686:F1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="F1:F680 F689:F691 F705:F1048576">
+    <cfRule type="duplicateValues" dxfId="23" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F530:F671">
-    <cfRule type="duplicateValues" dxfId="1" priority="308"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="329"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F681 F686:F1048576">
+  <conditionalFormatting sqref="F1:F681 F689:F691 F705:F1048576">
+    <cfRule type="duplicateValues" dxfId="21" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C689">
+    <cfRule type="duplicateValues" dxfId="20" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C689">
+    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C689">
+    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C689">
+    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C689">
+    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C689">
+    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C689">
+    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C690">
+    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C690">
+    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C690">
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C690">
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C690">
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C690">
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C690">
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C691">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C691">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C691">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C691">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C691">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C691">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C691">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C686" r:id="rId1" tooltip="Anopheles arabiensis (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Anopheles_arabiensis&amp;action=edit&amp;redlink=1" xr:uid="{80687BFB-0F94-0546-988E-BE85CD060F21}"/>
+    <hyperlink ref="C687" r:id="rId2" tooltip="Anopheles arabiensis (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Anopheles_arabiensis&amp;action=edit&amp;redlink=1" xr:uid="{BEBAA6D3-F881-D747-BCAA-C6E51422B7C3}"/>
+    <hyperlink ref="F686" r:id="rId3" tooltip="Anopheles arabiensis (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Anopheles_arabiensis&amp;action=edit&amp;redlink=1" xr:uid="{D3EE53A6-E12F-8C41-98CE-6679DF4456FD}"/>
+    <hyperlink ref="F687" r:id="rId4" tooltip="Anopheles arabiensis (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Anopheles_arabiensis&amp;action=edit&amp;redlink=1" xr:uid="{9D1BDE85-C848-6F40-B5DF-1A3B9766CC21}"/>
+    <hyperlink ref="C688" r:id="rId5" tooltip="Anopheles arabiensis (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Anopheles_arabiensis&amp;action=edit&amp;redlink=1" xr:uid="{DC316D98-5322-744C-A4A3-75521A6CF2E0}"/>
+    <hyperlink ref="F688" r:id="rId6" tooltip="Anopheles arabiensis (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Anopheles_arabiensis&amp;action=edit&amp;redlink=1" xr:uid="{E1F657BB-9E4B-0F4A-86F7-1332A89649F3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>